<commit_message>
Ajout gestion des filtres. Préparation sauvegarde des filtres.
</commit_message>
<xml_diff>
--- a/Exple-mouvements-BDD-Grands-Mécènes2.xlsx
+++ b/Exple-mouvements-BDD-Grands-Mécènes2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="213">
   <si>
     <t>Code délégué</t>
   </si>
@@ -659,6 +659,24 @@
   </si>
   <si>
     <t>01611245</t>
+  </si>
+  <si>
+    <t>Petit donateur</t>
+  </si>
+  <si>
+    <t>Moyen donateur</t>
+  </si>
+  <si>
+    <t>donateur nul</t>
+  </si>
+  <si>
+    <t>Atos</t>
+  </si>
+  <si>
+    <t>Amadeus</t>
+  </si>
+  <si>
+    <t>Monext</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1046,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,7 +1218,9 @@
       <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>46</v>
       </c>
@@ -1291,7 +1311,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>197</v>
@@ -1305,7 +1325,9 @@
       <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
@@ -1396,7 +1418,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>198</v>
@@ -1410,7 +1432,9 @@
       <c r="H4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1501,7 +1525,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>199</v>
@@ -1515,7 +1539,9 @@
       <c r="H5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1620,7 +1646,9 @@
       <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>46</v>
       </c>
@@ -1711,7 +1739,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>201</v>
@@ -1725,7 +1753,9 @@
       <c r="H7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1816,7 +1846,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>202</v>
@@ -1830,7 +1860,9 @@
       <c r="H8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1921,7 +1953,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>203</v>
@@ -1935,7 +1967,9 @@
       <c r="H9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2040,7 +2074,9 @@
       <c r="H10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>46</v>
       </c>
@@ -2131,7 +2167,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>205</v>
@@ -2145,7 +2181,9 @@
       <c r="H11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>46</v>
       </c>
@@ -2236,7 +2274,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>206</v>
@@ -2250,7 +2288,9 @@
       <c r="H12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>46</v>
       </c>
@@ -3327,7 +3367,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>193</v>
@@ -3341,7 +3381,9 @@
       <c r="H13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>46</v>
       </c>
@@ -3445,6 +3487,9 @@
       <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>46</v>
       </c>
@@ -3529,7 +3574,7 @@
         <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>61</v>
@@ -3542,6 +3587,9 @@
       </c>
       <c r="H15" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>64</v>
@@ -3618,7 +3666,7 @@
         <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>72</v>
@@ -3631,6 +3679,9 @@
       </c>
       <c r="H16" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -3707,7 +3758,7 @@
         <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>79</v>
@@ -3720,6 +3771,9 @@
       </c>
       <c r="H17" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>64</v>
@@ -3810,6 +3864,9 @@
       <c r="H18" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="I18" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>64</v>
       </c>
@@ -3885,7 +3942,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>91</v>
@@ -3898,6 +3955,9 @@
       </c>
       <c r="H19" s="1" t="s">
         <v>93</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>64</v>
@@ -3974,7 +4034,7 @@
         <v>96</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>97</v>
@@ -3987,6 +4047,9 @@
       </c>
       <c r="H20" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>64</v>
@@ -4063,7 +4126,7 @@
         <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>103</v>
@@ -4076,6 +4139,9 @@
       </c>
       <c r="H21" s="1" t="s">
         <v>105</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>64</v>
@@ -4166,6 +4232,9 @@
       <c r="H22" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="I22" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>64</v>
       </c>
@@ -4241,7 +4310,7 @@
         <v>114</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>115</v>
@@ -4254,6 +4323,9 @@
       </c>
       <c r="H23" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>64</v>
@@ -4330,7 +4402,7 @@
         <v>120</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>121</v>
@@ -4343,6 +4415,9 @@
       </c>
       <c r="H24" s="1" t="s">
         <v>123</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>64</v>
@@ -4419,7 +4494,7 @@
         <v>126</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>127</v>
@@ -4432,6 +4507,9 @@
       </c>
       <c r="H25" s="1" t="s">
         <v>129</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>64</v>
@@ -4522,6 +4600,9 @@
       <c r="H26" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="J26" s="1" t="s">
         <v>64</v>
       </c>
@@ -4597,7 +4678,7 @@
         <v>138</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>139</v>
@@ -4610,6 +4691,9 @@
       </c>
       <c r="H27" s="1" t="s">
         <v>141</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>64</v>
@@ -4686,7 +4770,7 @@
         <v>144</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>145</v>
@@ -4699,6 +4783,9 @@
       </c>
       <c r="H28" s="1" t="s">
         <v>147</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>64</v>
@@ -4775,7 +4862,7 @@
         <v>150</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>151</v>
@@ -4788,6 +4875,9 @@
       </c>
       <c r="H29" s="1" t="s">
         <v>153</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>64</v>
@@ -4878,6 +4968,9 @@
       <c r="H30" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="I30" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J30" s="1" t="s">
         <v>64</v>
       </c>
@@ -4953,7 +5046,7 @@
         <v>162</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>163</v>
@@ -4966,6 +5059,9 @@
       </c>
       <c r="H31" s="1" t="s">
         <v>165</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>64</v>
@@ -5042,7 +5138,7 @@
         <v>168</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>169</v>
@@ -5055,6 +5151,9 @@
       </c>
       <c r="H32" s="1" t="s">
         <v>171</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>64</v>
@@ -5131,7 +5230,7 @@
         <v>174</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>175</v>
@@ -5144,6 +5243,9 @@
       </c>
       <c r="H33" s="1" t="s">
         <v>177</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>64</v>
@@ -5234,6 +5336,9 @@
       <c r="H34" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="I34" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J34" s="1" t="s">
         <v>64</v>
       </c>
@@ -5322,6 +5427,9 @@
       </c>
       <c r="H35" s="1" t="s">
         <v>189</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>64</v>

</xml_diff>